<commit_message>
merge dict into single df
</commit_message>
<xml_diff>
--- a/data/UWS/_SO279_sampling_sheet.xlsx
+++ b/data/UWS/_SO279_sampling_sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://joinnioz-my.sharepoint.com/personal/louise_delaigue_nioz_nl/Documents/_DATA/SO279/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://joinnioz-my.sharepoint.com/personal/louise_delaigue_nioz_nl/Documents/_GITHUB/NAPTRAM2020/data/UWS/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{F3BCA63B-0657-4FFB-A86C-468AD2D326B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BC89D986-32D7-425D-8F61-3ED415AD77EE}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3D1C24D6-B482-4633-80E7-FE6A1A2CCD8F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{3D1C24D6-B482-4633-80E7-FE6A1A2CCD8F}"/>
   </bookViews>
   <sheets>
     <sheet name="sample_count" sheetId="3" r:id="rId1"/>
@@ -1434,9 +1434,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E656E55-4C50-4FC5-BBD3-EE98058A854C}">
   <dimension ref="A1:AC133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10294,8 +10294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB97071-ED23-40FB-9DE3-B17F032023BD}">
   <dimension ref="B2:I13"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
pyro data clean up
</commit_message>
<xml_diff>
--- a/data/UWS/_SO279_sampling_sheet.xlsx
+++ b/data/UWS/_SO279_sampling_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://joinnioz-my.sharepoint.com/personal/louise_delaigue_nioz_nl/Documents/_GITHUB/NAPTRAM2020/data/UWS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{F3BCA63B-0657-4FFB-A86C-468AD2D326B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BC89D986-32D7-425D-8F61-3ED415AD77EE}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{F3BCA63B-0657-4FFB-A86C-468AD2D326B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F45BBDF7-12FB-46FD-A755-F0DE588D38C6}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{3D1C24D6-B482-4633-80E7-FE6A1A2CCD8F}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="282">
   <si>
     <t>flag</t>
   </si>
@@ -267,9 +267,6 @@
     <t>CRM-189-0899</t>
   </si>
   <si>
-    <t>end of sampling period</t>
-  </si>
-  <si>
     <t>SO279_24-1_UWS</t>
   </si>
   <si>
@@ -411,24 +408,12 @@
     <t>file name</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>batch 1</t>
   </si>
   <si>
-    <t>naptram2020</t>
-  </si>
-  <si>
-    <t>naptram20202</t>
-  </si>
-  <si>
     <t>batch 3</t>
   </si>
   <si>
-    <t>naptram20203</t>
-  </si>
-  <si>
     <t>20 mL</t>
   </si>
   <si>
@@ -462,15 +447,9 @@
     <t>Stopped working on 18/12 at 11am because problem with pump</t>
   </si>
   <si>
-    <t>naptram20204</t>
-  </si>
-  <si>
     <t>didn’t recalibrate (seemed fine) + END: put in pH2 after 20/12 subsample at 16h50</t>
   </si>
   <si>
-    <t>naptram20205</t>
-  </si>
-  <si>
     <t>CRM-189-0225</t>
   </si>
   <si>
@@ -480,9 +459,6 @@
     <t>calibrated with last made buffers - had to end measurements as membrane pump needs maintenance // put optode in UWS seawater to not lose the calibration from previous night</t>
   </si>
   <si>
-    <t>naptram20206</t>
-  </si>
-  <si>
     <t>SO279_47-1_UWS</t>
   </si>
   <si>
@@ -789,18 +765,12 @@
     <t>didn't recalibrate as left optode in UWS seawater - after optode stabilization, values look fine 27/12 - 9h30ish, VTD turned the pump off without telling me - running a CRM6 as a sample to try and estimate drift</t>
   </si>
   <si>
-    <t>naptram2020CRM6</t>
-  </si>
-  <si>
     <t>see above line</t>
   </si>
   <si>
     <t>CRM-189-0530</t>
   </si>
   <si>
-    <t>naptram20207</t>
-  </si>
-  <si>
     <t>batch 4</t>
   </si>
   <si>
@@ -880,6 +850,42 @@
   </si>
   <si>
     <t>36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end of sampling period - skip from 1 day 1 hour 29 min to 1 day 1 hour 33 min (putting optode in CRM) + 33 min in, CRM until 40 min in (recalc value of CRM at the insitu value) + 40 min to 50 min optode in pH 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* WRONG TIMES, NEED TO CONVERT TO UTC (so - 1h) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-12-08_204002_SO279_STN1_test </t>
+  </si>
+  <si>
+    <t>2020-12-11_163148_NAPTRAM2020</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>2020-12-15_214136_NAPTRAM20202</t>
+  </si>
+  <si>
+    <t>2020-12-17_134828_NAPTRAM20203</t>
+  </si>
+  <si>
+    <t>2020-12-18_222759_NAPTRAM20204</t>
+  </si>
+  <si>
+    <t>2020-12-20_182318_NAPTRAM20205</t>
+  </si>
+  <si>
+    <t>2020-12-21_112915_NAPTRAM20206</t>
+  </si>
+  <si>
+    <t>2020-12-28_151321_NAPTRAM20207</t>
+  </si>
+  <si>
+    <t>2020-12-27_101200_NAPTRAM2020CRM6</t>
   </si>
 </sst>
 </file>
@@ -889,7 +895,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -907,6 +913,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -944,7 +957,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -992,6 +1005,13 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1323,19 +1343,19 @@
         <v>34</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C4">
         <f>SUM(sampling_sheet!R5:R154)</f>
         <v>255</v>
       </c>
       <c r="E4" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="F4">
         <f>SUM(sampling_sheet!V5:V154)</f>
@@ -1344,14 +1364,14 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="C5">
         <f>SUM(sampling_sheet!U5:U192)</f>
         <v>256</v>
       </c>
       <c r="E5" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="F5">
         <f>SUM(sampling_sheet!W5:W155)</f>
@@ -1360,14 +1380,14 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C6">
         <f>SUM(sampling_sheet!T5:T193)</f>
         <v>256</v>
       </c>
       <c r="E6" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F6">
         <f>SUM(sampling_sheet!X5:X156)</f>
@@ -1376,14 +1396,14 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="C7">
         <f>SUM(sampling_sheet!S5:S194)</f>
         <v>256</v>
       </c>
       <c r="E7" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="F7">
         <f>SUM(sampling_sheet!Y5:Y157)</f>
@@ -1392,7 +1412,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="F8">
         <f>SUM(sampling_sheet!Z5:Z158)</f>
@@ -1401,7 +1421,7 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="C10" s="5">
         <f>SUM(C4:C7)</f>
@@ -1417,7 +1437,7 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F11" s="5">
         <f>SUM(C10+F10)</f>
@@ -1526,13 +1546,13 @@
         <v>12</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="Y1" s="5" t="s">
         <v>33</v>
@@ -1655,19 +1675,19 @@
         <v>34</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AB3" s="8"/>
     </row>
@@ -1681,31 +1701,31 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="R4" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="AB4" s="8"/>
     </row>
@@ -2626,7 +2646,7 @@
         <v>9</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K19" s="11">
         <v>10</v>
@@ -2700,7 +2720,7 @@
         <v>14</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>38</v>
@@ -2836,7 +2856,7 @@
         <v>12</v>
       </c>
       <c r="J22" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K22" s="11">
         <v>27</v>
@@ -3019,7 +3039,7 @@
         <v>34</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>32</v>
@@ -3046,7 +3066,7 @@
         <v>22</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>38</v>
@@ -3088,7 +3108,7 @@
         <v>34</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>32</v>
@@ -3149,7 +3169,7 @@
         <v>34</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>32</v>
@@ -3210,7 +3230,7 @@
         <v>34</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>32</v>
@@ -3271,7 +3291,7 @@
         <v>34</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>32</v>
@@ -3332,7 +3352,7 @@
         <v>34</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>32</v>
@@ -3393,7 +3413,7 @@
         <v>34</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>32</v>
@@ -3454,7 +3474,7 @@
         <v>34</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>32</v>
@@ -3515,7 +3535,7 @@
         <v>34</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>32</v>
@@ -3576,7 +3596,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>32</v>
@@ -3637,7 +3657,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>32</v>
@@ -3698,7 +3718,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>32</v>
@@ -3759,7 +3779,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>32</v>
@@ -3783,7 +3803,7 @@
         <v>14</v>
       </c>
       <c r="J37" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K37" s="11">
         <v>28</v>
@@ -3822,7 +3842,7 @@
         <v>0</v>
       </c>
       <c r="AB37" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.25">
@@ -3830,7 +3850,7 @@
         <v>34</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>32</v>
@@ -3854,10 +3874,10 @@
         <v>15</v>
       </c>
       <c r="J38" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="K38" s="11" t="s">
         <v>94</v>
-      </c>
-      <c r="K38" s="11" t="s">
-        <v>95</v>
       </c>
       <c r="L38" s="2" t="s">
         <v>38</v>
@@ -3893,7 +3913,7 @@
         <v>0</v>
       </c>
       <c r="AB38" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.25">
@@ -3901,7 +3921,7 @@
         <v>34</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>32</v>
@@ -3962,7 +3982,7 @@
         <v>34</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>32</v>
@@ -4018,7 +4038,7 @@
         <v>0</v>
       </c>
       <c r="AB40" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.25">
@@ -4026,7 +4046,7 @@
         <v>34</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>32</v>
@@ -4087,7 +4107,7 @@
         <v>34</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>32</v>
@@ -4143,7 +4163,7 @@
         <v>0</v>
       </c>
       <c r="AB42" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.25">
@@ -4151,7 +4171,7 @@
         <v>34</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>32</v>
@@ -4212,7 +4232,7 @@
         <v>34</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>32</v>
@@ -4273,7 +4293,7 @@
         <v>34</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>32</v>
@@ -4338,7 +4358,7 @@
         <v>34</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>32</v>
@@ -4399,7 +4419,7 @@
         <v>34</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>32</v>
@@ -4460,7 +4480,7 @@
         <v>34</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>32</v>
@@ -4521,7 +4541,7 @@
         <v>34</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>32</v>
@@ -4545,10 +4565,10 @@
         <v>16</v>
       </c>
       <c r="J49" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="K49" s="11" t="s">
         <v>108</v>
-      </c>
-      <c r="K49" s="11" t="s">
-        <v>109</v>
       </c>
       <c r="L49" s="2" t="s">
         <v>38</v>
@@ -4584,7 +4604,7 @@
         <v>0</v>
       </c>
       <c r="AB49" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:28" x14ac:dyDescent="0.25">
@@ -4592,7 +4612,7 @@
         <v>34</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>32</v>
@@ -4616,10 +4636,10 @@
         <v>17</v>
       </c>
       <c r="J50" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="K50" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="K50" s="11" t="s">
-        <v>114</v>
       </c>
       <c r="L50" s="2" t="s">
         <v>38</v>
@@ -4655,7 +4675,7 @@
         <v>0</v>
       </c>
       <c r="AB50" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:28" x14ac:dyDescent="0.25">
@@ -4663,7 +4683,7 @@
         <v>34</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>32</v>
@@ -4731,7 +4751,7 @@
         <v>34</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>32</v>
@@ -4799,7 +4819,7 @@
         <v>34</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>32</v>
@@ -4860,7 +4880,7 @@
         <v>34</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>32</v>
@@ -4921,7 +4941,7 @@
         <v>34</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>32</v>
@@ -4982,7 +5002,7 @@
         <v>34</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>32</v>
@@ -5043,7 +5063,7 @@
         <v>34</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>32</v>
@@ -5104,7 +5124,7 @@
         <v>34</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>32</v>
@@ -5165,7 +5185,7 @@
         <v>34</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>32</v>
@@ -5226,7 +5246,7 @@
         <v>34</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>32</v>
@@ -5287,7 +5307,7 @@
         <v>34</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>32</v>
@@ -5348,7 +5368,7 @@
         <v>34</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>32</v>
@@ -5409,7 +5429,7 @@
         <v>34</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>32</v>
@@ -5470,7 +5490,7 @@
         <v>34</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>32</v>
@@ -5538,7 +5558,7 @@
         <v>34</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>32</v>
@@ -5601,7 +5621,7 @@
         <v>0</v>
       </c>
       <c r="AB65" s="6" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="66" spans="1:29" x14ac:dyDescent="0.25">
@@ -5609,7 +5629,7 @@
         <v>34</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>32</v>
@@ -5672,7 +5692,7 @@
         <v>0</v>
       </c>
       <c r="AB66" s="6" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="67" spans="1:29" x14ac:dyDescent="0.25">
@@ -5680,7 +5700,7 @@
         <v>34</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>32</v>
@@ -5743,7 +5763,7 @@
         <v>0</v>
       </c>
       <c r="AB67" s="6" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="68" spans="1:29" x14ac:dyDescent="0.25">
@@ -5751,7 +5771,7 @@
         <v>34</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>32</v>
@@ -5814,7 +5834,7 @@
         <v>0</v>
       </c>
       <c r="AB68" s="6" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="69" spans="1:29" x14ac:dyDescent="0.25">
@@ -5822,7 +5842,7 @@
         <v>34</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>32</v>
@@ -5885,7 +5905,7 @@
         <v>0</v>
       </c>
       <c r="AB69" s="6" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="70" spans="1:29" x14ac:dyDescent="0.25">
@@ -5893,7 +5913,7 @@
         <v>34</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>32</v>
@@ -5920,7 +5940,7 @@
         <v>22</v>
       </c>
       <c r="K70" s="11" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="L70" s="2" t="s">
         <v>38</v>
@@ -5961,7 +5981,7 @@
         <v>34</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>32</v>
@@ -5988,7 +6008,7 @@
         <v>9</v>
       </c>
       <c r="K71" s="11" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="L71" s="2" t="s">
         <v>38</v>
@@ -6029,7 +6049,7 @@
         <v>34</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>32</v>
@@ -6090,7 +6110,7 @@
         <v>34</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>32</v>
@@ -6151,7 +6171,7 @@
         <v>34</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>32</v>
@@ -6212,7 +6232,7 @@
         <v>34</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>32</v>
@@ -6277,7 +6297,7 @@
         <v>34</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>32</v>
@@ -6338,7 +6358,7 @@
         <v>34</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>32</v>
@@ -6399,7 +6419,7 @@
         <v>34</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>32</v>
@@ -6460,7 +6480,7 @@
         <v>34</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>32</v>
@@ -6521,7 +6541,7 @@
         <v>34</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>32</v>
@@ -6582,7 +6602,7 @@
         <v>34</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>32</v>
@@ -6643,7 +6663,7 @@
         <v>34</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>32</v>
@@ -6704,7 +6724,7 @@
         <v>34</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>32</v>
@@ -6731,7 +6751,7 @@
         <v>16</v>
       </c>
       <c r="K83" s="11" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="L83" s="2" t="s">
         <v>38</v>
@@ -6772,7 +6792,7 @@
         <v>34</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>32</v>
@@ -6799,7 +6819,7 @@
         <v>22</v>
       </c>
       <c r="K84" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L84" s="2" t="s">
         <v>38</v>
@@ -6840,7 +6860,7 @@
         <v>34</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>32</v>
@@ -6867,7 +6887,7 @@
         <v>9</v>
       </c>
       <c r="K85" s="11" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="L85" s="2" t="s">
         <v>38</v>
@@ -6908,7 +6928,7 @@
         <v>34</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>32</v>
@@ -6935,7 +6955,7 @@
         <v>11</v>
       </c>
       <c r="K86" s="11" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="L86" s="2" t="s">
         <v>38</v>
@@ -6976,7 +6996,7 @@
         <v>34</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>32</v>
@@ -7037,7 +7057,7 @@
         <v>34</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>32</v>
@@ -7098,7 +7118,7 @@
         <v>34</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>32</v>
@@ -7159,7 +7179,7 @@
         <v>34</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>32</v>
@@ -7220,7 +7240,7 @@
         <v>34</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>32</v>
@@ -7281,7 +7301,7 @@
         <v>34</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>32</v>
@@ -7342,7 +7362,7 @@
         <v>34</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>32</v>
@@ -7403,7 +7423,7 @@
         <v>34</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>32</v>
@@ -7464,7 +7484,7 @@
         <v>34</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>32</v>
@@ -7525,7 +7545,7 @@
         <v>34</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>32</v>
@@ -7586,7 +7606,7 @@
         <v>34</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>32</v>
@@ -7642,7 +7662,7 @@
         <v>0</v>
       </c>
       <c r="AB97" s="6" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="98" spans="1:28" x14ac:dyDescent="0.25">
@@ -7650,7 +7670,7 @@
         <v>34</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>32</v>
@@ -7677,7 +7697,7 @@
         <v>21</v>
       </c>
       <c r="K98" s="11" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="L98" s="2" t="s">
         <v>38</v>
@@ -7718,7 +7738,7 @@
         <v>34</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>32</v>
@@ -7745,7 +7765,7 @@
         <v>10</v>
       </c>
       <c r="K99" s="11" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="L99" s="2" t="s">
         <v>38</v>
@@ -7786,7 +7806,7 @@
         <v>34</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>32</v>
@@ -7813,7 +7833,7 @@
         <v>21</v>
       </c>
       <c r="K100" s="11" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="L100" s="2" t="s">
         <v>38</v>
@@ -7854,7 +7874,7 @@
         <v>34</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>32</v>
@@ -7881,7 +7901,7 @@
         <v>11</v>
       </c>
       <c r="K101" s="11" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="L101" s="2" t="s">
         <v>38</v>
@@ -7917,7 +7937,7 @@
         <v>0</v>
       </c>
       <c r="AB101" s="6" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="102" spans="1:28" x14ac:dyDescent="0.25">
@@ -7925,7 +7945,7 @@
         <v>34</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>32</v>
@@ -7952,7 +7972,7 @@
         <v>21</v>
       </c>
       <c r="K102" s="11" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="L102" s="2" t="s">
         <v>38</v>
@@ -7988,7 +8008,7 @@
         <v>0</v>
       </c>
       <c r="AB102" s="6" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="103" spans="1:28" x14ac:dyDescent="0.25">
@@ -7996,7 +8016,7 @@
         <v>34</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>32</v>
@@ -8023,7 +8043,7 @@
         <v>10</v>
       </c>
       <c r="K103" s="11" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="L103" s="2" t="s">
         <v>38</v>
@@ -8059,7 +8079,7 @@
         <v>0</v>
       </c>
       <c r="AB103" s="6" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="104" spans="1:28" x14ac:dyDescent="0.25">
@@ -8067,7 +8087,7 @@
         <v>34</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>32</v>
@@ -8094,7 +8114,7 @@
         <v>23</v>
       </c>
       <c r="K104" s="11" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="L104" s="2" t="s">
         <v>38</v>
@@ -8130,7 +8150,7 @@
         <v>0</v>
       </c>
       <c r="AB104" s="6" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="105" spans="1:28" x14ac:dyDescent="0.25">
@@ -8138,7 +8158,7 @@
         <v>34</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>32</v>
@@ -8165,7 +8185,7 @@
         <v>11</v>
       </c>
       <c r="K105" s="11" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="L105" s="2" t="s">
         <v>38</v>
@@ -8201,7 +8221,7 @@
         <v>0</v>
       </c>
       <c r="AB105" s="6" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="106" spans="1:28" x14ac:dyDescent="0.25">
@@ -8209,7 +8229,7 @@
         <v>34</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>32</v>
@@ -8236,7 +8256,7 @@
         <v>21</v>
       </c>
       <c r="K106" s="11" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="L106" s="2" t="s">
         <v>38</v>
@@ -8272,7 +8292,7 @@
         <v>0</v>
       </c>
       <c r="AB106" s="6" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="107" spans="1:28" x14ac:dyDescent="0.25">
@@ -8280,7 +8300,7 @@
         <v>34</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>32</v>
@@ -8307,7 +8327,7 @@
         <v>10</v>
       </c>
       <c r="K107" s="11" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="L107" s="2" t="s">
         <v>38</v>
@@ -8343,7 +8363,7 @@
         <v>0</v>
       </c>
       <c r="AB107" s="6" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="108" spans="1:28" x14ac:dyDescent="0.25">
@@ -8351,7 +8371,7 @@
         <v>34</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>32</v>
@@ -8378,7 +8398,7 @@
         <v>22</v>
       </c>
       <c r="K108" s="11" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="L108" s="2" t="s">
         <v>38</v>
@@ -8414,7 +8434,7 @@
         <v>0</v>
       </c>
       <c r="AB108" s="6" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
     </row>
     <row r="109" spans="1:28" x14ac:dyDescent="0.25">
@@ -8422,7 +8442,7 @@
         <v>34</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>32</v>
@@ -8483,7 +8503,7 @@
         <v>34</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>32</v>
@@ -8544,7 +8564,7 @@
         <v>34</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>32</v>
@@ -8605,7 +8625,7 @@
         <v>34</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>32</v>
@@ -8666,7 +8686,7 @@
         <v>34</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C113" s="3" t="s">
         <v>32</v>
@@ -8727,7 +8747,7 @@
         <v>34</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>32</v>
@@ -8788,7 +8808,7 @@
         <v>34</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>32</v>
@@ -8849,7 +8869,7 @@
         <v>34</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>32</v>
@@ -8910,7 +8930,7 @@
         <v>34</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="C117" s="3" t="s">
         <v>32</v>
@@ -8971,7 +8991,7 @@
         <v>34</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C118" s="3" t="s">
         <v>32</v>
@@ -9032,7 +9052,7 @@
         <v>34</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>32</v>
@@ -9093,7 +9113,7 @@
         <v>34</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>32</v>
@@ -9120,7 +9140,7 @@
         <v>15</v>
       </c>
       <c r="K120" s="11" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="L120" s="2" t="s">
         <v>38</v>
@@ -9161,7 +9181,7 @@
         <v>34</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>32</v>
@@ -9188,7 +9208,7 @@
         <v>21</v>
       </c>
       <c r="K121" s="11" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="L121" s="2" t="s">
         <v>38</v>
@@ -9224,7 +9244,7 @@
         <v>0</v>
       </c>
       <c r="AB121" s="6" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="122" spans="1:28" x14ac:dyDescent="0.25">
@@ -9232,7 +9252,7 @@
         <v>34</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="C122" s="3" t="s">
         <v>32</v>
@@ -9259,7 +9279,7 @@
         <v>10</v>
       </c>
       <c r="K122" s="11" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="L122" s="2" t="s">
         <v>38</v>
@@ -9295,7 +9315,7 @@
         <v>0</v>
       </c>
       <c r="AB122" s="6" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="123" spans="1:28" x14ac:dyDescent="0.25">
@@ -9303,7 +9323,7 @@
         <v>34</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="C123" s="3" t="s">
         <v>32</v>
@@ -9330,7 +9350,7 @@
         <v>22</v>
       </c>
       <c r="K123" s="11" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="L123" s="2" t="s">
         <v>38</v>
@@ -9366,7 +9386,7 @@
         <v>0</v>
       </c>
       <c r="AB123" s="6" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="124" spans="1:28" x14ac:dyDescent="0.25">
@@ -9374,7 +9394,7 @@
         <v>34</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="C124" s="3" t="s">
         <v>32</v>
@@ -9401,7 +9421,7 @@
         <v>12</v>
       </c>
       <c r="K124" s="11" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="L124" s="2" t="s">
         <v>38</v>
@@ -9437,7 +9457,7 @@
         <v>0</v>
       </c>
       <c r="AB124" s="6" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="125" spans="1:28" x14ac:dyDescent="0.25">
@@ -9445,7 +9465,7 @@
         <v>34</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="C125" s="3" t="s">
         <v>32</v>
@@ -9472,7 +9492,7 @@
         <v>19</v>
       </c>
       <c r="K125" s="11" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="L125" s="2" t="s">
         <v>38</v>
@@ -9508,7 +9528,7 @@
         <v>0</v>
       </c>
       <c r="AB125" s="6" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="126" spans="1:28" x14ac:dyDescent="0.25">
@@ -9516,7 +9536,7 @@
         <v>34</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>32</v>
@@ -9543,7 +9563,7 @@
         <v>19</v>
       </c>
       <c r="K126" s="11" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="L126" s="2" t="s">
         <v>38</v>
@@ -9579,7 +9599,7 @@
         <v>0</v>
       </c>
       <c r="AB126" s="6" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="127" spans="1:28" x14ac:dyDescent="0.25">
@@ -9587,7 +9607,7 @@
         <v>34</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="C127" s="3" t="s">
         <v>32</v>
@@ -9614,7 +9634,7 @@
         <v>20</v>
       </c>
       <c r="K127" s="11" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="L127" s="2" t="s">
         <v>38</v>
@@ -9650,7 +9670,7 @@
         <v>0</v>
       </c>
       <c r="AB127" s="6" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="128" spans="1:28" x14ac:dyDescent="0.25">
@@ -9658,7 +9678,7 @@
         <v>34</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>32</v>
@@ -9685,7 +9705,7 @@
         <v>20</v>
       </c>
       <c r="K128" s="11" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="L128" s="2" t="s">
         <v>38</v>
@@ -9721,7 +9741,7 @@
         <v>0</v>
       </c>
       <c r="AB128" s="6" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="129" spans="1:28" x14ac:dyDescent="0.25">
@@ -9729,7 +9749,7 @@
         <v>34</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>32</v>
@@ -9756,7 +9776,7 @@
         <v>20</v>
       </c>
       <c r="K129" s="11" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="L129" s="2" t="s">
         <v>38</v>
@@ -9792,7 +9812,7 @@
         <v>0</v>
       </c>
       <c r="AB129" s="6" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="130" spans="1:28" x14ac:dyDescent="0.25">
@@ -9800,7 +9820,7 @@
         <v>34</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>32</v>
@@ -9827,7 +9847,7 @@
         <v>20</v>
       </c>
       <c r="K130" s="11" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="L130" s="2" t="s">
         <v>38</v>
@@ -9863,7 +9883,7 @@
         <v>0</v>
       </c>
       <c r="AB130" s="6" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="131" spans="1:28" x14ac:dyDescent="0.25">
@@ -9871,7 +9891,7 @@
         <v>34</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="C131" s="3" t="s">
         <v>32</v>
@@ -9898,7 +9918,7 @@
         <v>21</v>
       </c>
       <c r="K131" s="11" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="L131" s="2" t="s">
         <v>38</v>
@@ -9934,7 +9954,7 @@
         <v>0</v>
       </c>
       <c r="AB131" s="6" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="132" spans="1:28" x14ac:dyDescent="0.25">
@@ -9942,7 +9962,7 @@
         <v>34</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>32</v>
@@ -9969,7 +9989,7 @@
         <v>21</v>
       </c>
       <c r="K132" s="11" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="L132" s="2" t="s">
         <v>38</v>
@@ -10005,7 +10025,7 @@
         <v>0</v>
       </c>
       <c r="AB132" s="6" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="133" spans="1:28" x14ac:dyDescent="0.25">
@@ -10013,7 +10033,7 @@
         <v>34</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>32</v>
@@ -10040,7 +10060,7 @@
         <v>21</v>
       </c>
       <c r="K133" s="11" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="L133" s="2" t="s">
         <v>38</v>
@@ -10076,7 +10096,7 @@
         <v>0</v>
       </c>
       <c r="AB133" s="6" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -10140,7 +10160,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G2" s="11">
         <v>10</v>
@@ -10166,7 +10186,7 @@
         <v>14</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -10209,7 +10229,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G5" s="11">
         <v>27</v>
@@ -10266,7 +10286,7 @@
         <v>34</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" s="2">
         <v>2020</v>
@@ -10281,7 +10301,7 @@
         <v>22</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -10292,45 +10312,48 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB97071-ED23-40FB-9DE3-B17F032023BD}">
-  <dimension ref="B2:I13"/>
+  <dimension ref="A2:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E2" t="s">
         <v>72</v>
       </c>
       <c r="F2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>274</v>
+      </c>
       <c r="B3" s="10">
         <v>44173</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>123</v>
+      <c r="C3" s="18" t="s">
+        <v>272</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E3" t="s">
         <v>70</v>
@@ -10339,32 +10362,35 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>274</v>
+      </c>
       <c r="B4" s="10">
         <v>44174</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>123</v>
+      <c r="C4" s="18" t="s">
+        <v>272</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E4" t="s">
         <v>74</v>
       </c>
       <c r="F4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="10">
         <v>44176</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>125</v>
+      <c r="C5" s="18" t="s">
+        <v>273</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E5" t="s">
         <v>63</v>
@@ -10373,55 +10399,55 @@
         <v>73</v>
       </c>
       <c r="I5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="10">
         <v>44180</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>126</v>
+      <c r="C6" s="18" t="s">
+        <v>275</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F6" t="s">
         <v>73</v>
       </c>
       <c r="I6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="10">
         <v>44182</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>128</v>
+      <c r="C7" s="18" t="s">
+        <v>276</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F7" t="s">
         <v>73</v>
       </c>
       <c r="I7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <v>44183</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>140</v>
+      <c r="C8" s="18" t="s">
+        <v>277</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>66</v>
@@ -10430,29 +10456,29 @@
         <v>66</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="10" t="s">
-        <v>142</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="18" t="s">
+        <v>278</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E9" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="F9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="10">
         <v>44186</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>146</v>
+      <c r="C10" s="18" t="s">
+        <v>279</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>66</v>
@@ -10461,47 +10487,53 @@
         <v>66</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>44192</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>249</v>
+      <c r="C11" s="18" t="s">
+        <v>281</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <v>44193</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>252</v>
+      <c r="C12" s="18" t="s">
+        <v>280</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="E12" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="19" t="s">
+        <v>271</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>